<commit_message>
update mobile release note
</commit_message>
<xml_diff>
--- a/mCovid Plan Mobile.xlsx
+++ b/mCovid Plan Mobile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lengocthanhnhan/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lengocthanhnhan/Desktop/NMB/MCOVID/mcovid-docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B17B6C7-9B51-F440-BC49-E2DC134605BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C99B6E-D355-0545-98AB-E3045F8001AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6780" yWindow="1000" windowWidth="32180" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1640" yWindow="460" windowWidth="31960" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="hidden" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="79">
   <si>
     <t>Project</t>
   </si>
@@ -140,24 +140,12 @@
     <t>Grand Total</t>
   </si>
   <si>
-    <t>Dashboard</t>
-  </si>
-  <si>
-    <t>NXSON</t>
-  </si>
-  <si>
     <t>Edoc Mobile</t>
   </si>
   <si>
     <t>React Native</t>
   </si>
   <si>
-    <t>Nguyễn Xuân Sơn</t>
-  </si>
-  <si>
-    <t>Fixbug</t>
-  </si>
-  <si>
     <t>%Complete</t>
   </si>
   <si>
@@ -173,133 +161,121 @@
     <t>Knowledge Library</t>
   </si>
   <si>
-    <t>Forums</t>
-  </si>
-  <si>
-    <t>Users</t>
-  </si>
-  <si>
-    <t>Administrator</t>
-  </si>
-  <si>
     <t>Notification</t>
   </si>
   <si>
-    <t>Setting</t>
-  </si>
-  <si>
-    <t>Architect</t>
-  </si>
-  <si>
-    <t>Layout</t>
-  </si>
-  <si>
-    <t>Definition Language</t>
-  </si>
-  <si>
     <t>Login</t>
   </si>
   <si>
-    <t>Logout</t>
-  </si>
-  <si>
-    <t>Genarate Data</t>
-  </si>
-  <si>
-    <t>DDMINH</t>
-  </si>
-  <si>
-    <t>Đỗ Đức Minh</t>
-  </si>
-  <si>
-    <t>Paging</t>
-  </si>
-  <si>
-    <t>Display Detail</t>
-  </si>
-  <si>
-    <t>Display List + Paging</t>
-  </si>
-  <si>
-    <t>CRUD Post</t>
-  </si>
-  <si>
     <t>Display List Module</t>
   </si>
   <si>
     <t>Detail Module</t>
   </si>
   <si>
-    <t>Filter</t>
-  </si>
-  <si>
-    <t>Display Capsules</t>
-  </si>
-  <si>
-    <t>Detail Capsule</t>
-  </si>
-  <si>
-    <t>Filter Capsule</t>
-  </si>
-  <si>
-    <t>Display Capsule Rate</t>
-  </si>
-  <si>
     <t>List Knowledge Module</t>
   </si>
   <si>
     <t>Detail Knowledge</t>
   </si>
   <si>
-    <t>CRUD Knowledge</t>
-  </si>
-  <si>
-    <t>CRUD Knowledge Category</t>
-  </si>
-  <si>
-    <t>CRUD Knowledge Document</t>
-  </si>
-  <si>
-    <t>List Forum</t>
-  </si>
-  <si>
-    <t>Detail Forum</t>
-  </si>
-  <si>
-    <t>CRUD Forum</t>
-  </si>
-  <si>
-    <t>List User</t>
-  </si>
-  <si>
-    <t>Update User</t>
-  </si>
-  <si>
-    <t>List Administrator Accounts</t>
-  </si>
-  <si>
-    <t>Update Administrator Account</t>
-  </si>
-  <si>
-    <t>Roles</t>
-  </si>
-  <si>
-    <t>CRUD Role</t>
-  </si>
-  <si>
-    <t>Notificate template</t>
-  </si>
-  <si>
-    <t>CRUD Notification template</t>
-  </si>
-  <si>
-    <t>Import Account from excel</t>
-  </si>
-  <si>
-    <t>Update site setting</t>
-  </si>
-  <si>
-    <t>Site langugae</t>
+    <t>Nguyễn Đình Thắng</t>
+  </si>
+  <si>
+    <t>New feed</t>
+  </si>
+  <si>
+    <t>Display newfeed</t>
+  </si>
+  <si>
+    <t>Post Text</t>
+  </si>
+  <si>
+    <t>Post Image</t>
+  </si>
+  <si>
+    <t>Like</t>
+  </si>
+  <si>
+    <t>Share</t>
+  </si>
+  <si>
+    <t>NDTHANG</t>
+  </si>
+  <si>
+    <t>Enrol module</t>
+  </si>
+  <si>
+    <t>Display Recommendation</t>
+  </si>
+  <si>
+    <t>Display Learning history</t>
+  </si>
+  <si>
+    <t>Favarite</t>
+  </si>
+  <si>
+    <t>Dowload</t>
+  </si>
+  <si>
+    <t>My Network</t>
+  </si>
+  <si>
+    <t>My Post</t>
+  </si>
+  <si>
+    <t>My Friend</t>
+  </si>
+  <si>
+    <t>My Forums</t>
+  </si>
+  <si>
+    <t>Pofile</t>
+  </si>
+  <si>
+    <t>Update profile</t>
+  </si>
+  <si>
+    <t>Update password</t>
+  </si>
+  <si>
+    <t>My Dashboard</t>
+  </si>
+  <si>
+    <t>Download</t>
+  </si>
+  <si>
+    <t>List notification</t>
+  </si>
+  <si>
+    <t>Authenticate</t>
+  </si>
+  <si>
+    <t>Intro</t>
+  </si>
+  <si>
+    <t>Display intro screen</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>Login by Linkedin</t>
+  </si>
+  <si>
+    <t>Login by Twitter</t>
+  </si>
+  <si>
+    <t>Display users like</t>
+  </si>
+  <si>
+    <t>Post video</t>
+  </si>
+  <si>
+    <t>Post link</t>
+  </si>
+  <si>
+    <t>Detaile newfeed</t>
   </si>
 </sst>
 </file>
@@ -444,7 +420,148 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="39">
+  <dxfs count="40">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="ddd\ dd/mm/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -463,147 +580,6 @@
       </font>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="ddd\ dd/mm/yyyy"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -791,6 +767,11 @@
         <horizontal/>
       </border>
       <protection locked="0" hidden="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -2028,7 +2009,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="No.">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="No.">
   <location ref="C9:E25" firstHeaderRow="1" firstDataRow="1" firstDataCol="3"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -2247,7 +2228,7 @@
     <i/>
   </colItems>
   <formats count="1">
-    <format dxfId="38">
+    <format dxfId="39">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="7" count="0"/>
@@ -2268,28 +2249,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="tblPlan" displayName="tblPlan" ref="A1:K50" totalsRowCount="1" headerRowDxfId="37" dataDxfId="36" totalsRowDxfId="34" tableBorderDxfId="35">
-  <autoFilter ref="A1:K49" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="tblPlan" displayName="tblPlan" ref="A1:K47" totalsRowCount="1" headerRowDxfId="38" dataDxfId="37" totalsRowDxfId="35" tableBorderDxfId="36">
+  <autoFilter ref="A1:K46" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Lv1." totalsRowLabel="Finish" dataDxfId="24" totalsRowDxfId="13">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Lv1." totalsRowLabel="Finish" dataDxfId="24" totalsRowDxfId="10">
       <calculatedColumnFormula>COUNTA(OFFSET(tblPlan[[#Headers],[Task]],1,0,ROW()-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Lv2." dataDxfId="23" totalsRowDxfId="12">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Lv2." dataDxfId="23" totalsRowDxfId="9">
       <calculatedColumnFormula>IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="No." dataDxfId="22" totalsRowDxfId="11">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="No." dataDxfId="22" totalsRowDxfId="8">
       <calculatedColumnFormula>IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Task" dataDxfId="21" totalsRowDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Detail" dataDxfId="20" totalsRowDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Efforts(mds)" dataDxfId="19" totalsRowDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Start" dataDxfId="18" totalsRowDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Finish" totalsRowFunction="max" dataDxfId="17" totalsRowDxfId="6">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Task" dataDxfId="21" totalsRowDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Detail" dataDxfId="20" totalsRowDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Efforts(mds)" dataDxfId="19" totalsRowDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Start" dataDxfId="18" totalsRowDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Finish" totalsRowFunction="max" dataDxfId="17" totalsRowDxfId="3">
       <calculatedColumnFormula>IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",MAX(OFFSET(tblPlan[[#This Row],[Start]],1,1,COUNTIF(tblPlan[Lv1.],tblPlan[[#This Row],[Lv1.]])-1)),IF(tblPlan[[#This Row],[Start]]&lt;&gt;"",WORKDAY.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Efforts(mds)]]-NETWORKDAYS.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Start]],11,tblHoliday[Date]),11,tblHoliday[Date]),""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Resource" dataDxfId="16" totalsRowDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="%Complete" dataDxfId="15" totalsRowDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Comment" dataDxfId="14" totalsRowDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Resource" dataDxfId="16" totalsRowDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="%Complete" dataDxfId="15" totalsRowDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Comment" dataDxfId="14" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2299,24 +2280,24 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="tblHoliday" displayName="tblHoliday" ref="A1:C3" totalsRowShown="0">
   <autoFilter ref="A1:C3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="No." dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Date" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="No." dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Date" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="tblResources" displayName="tblResources" ref="A1:D4" totalsRowShown="0" headerRowDxfId="30" tableBorderDxfId="29">
-  <autoFilter ref="A1:D4" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="tblResources" displayName="tblResources" ref="A1:D3" totalsRowShown="0" headerRowDxfId="31" tableBorderDxfId="30">
+  <autoFilter ref="A1:D3" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="No." dataDxfId="28">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="No." dataDxfId="29">
       <calculatedColumnFormula>ROW()-ROW(tblResources[[#Headers],[No.]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Account" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Fullname" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Description" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Account" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Fullname" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Description" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2605,7 +2586,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2613,7 +2594,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2830,10 +2811,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C46" sqref="A46:XFD46"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2876,30 +2857,30 @@
         <v>9</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K1" s="10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="11">
+      <c r="A2" s="21">
         <f ca="1">COUNTA(OFFSET(tblPlan[[#Headers],[Task]],1,0,ROW()-1))</f>
         <v>1</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="22">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
         <v>0</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="23">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
         <v>1</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
@@ -2913,21 +2894,21 @@
       <c r="K2" s="24"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="11">
+      <c r="A3" s="21">
         <f ca="1">COUNTA(OFFSET(tblPlan[[#Headers],[Task]],1,0,ROW()-1))</f>
         <v>1</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="22">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
         <v>1</v>
       </c>
-      <c r="C3" s="13" t="str">
+      <c r="C3" s="23" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
         <v>1.1</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="14"/>
@@ -2939,57 +2920,53 @@
         <v>29</v>
       </c>
       <c r="J3" s="26">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="K3" s="24"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <f ca="1">COUNTA(OFFSET(tblPlan[[#Headers],[Task]],1,0,ROW()-1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="12">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="13">
+        <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
         <v>2</v>
       </c>
-      <c r="C4" s="13" t="str">
-        <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>1.2</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9" t="s">
-        <v>51</v>
-      </c>
+      <c r="D4" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="14"/>
-      <c r="H4" s="15" t="str">
+      <c r="H4" s="15">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",MAX(OFFSET(tblPlan[[#This Row],[Start]],1,1,COUNTIF(tblPlan[Lv1.],tblPlan[[#This Row],[Lv1.]])-1)),IF(tblPlan[[#This Row],[Start]]&lt;&gt;"",WORKDAY.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Efforts(mds)]]-NETWORKDAYS.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Start]],11,tblHoliday[Date]),11,tblHoliday[Date]),""))</f>
-        <v/>
-      </c>
-      <c r="I4" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="26">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I4" s="16"/>
+      <c r="J4" s="26"/>
       <c r="K4" s="24"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <f ca="1">COUNTA(OFFSET(tblPlan[[#Headers],[Task]],1,0,ROW()-1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" s="12">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" s="13" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>1.3</v>
+        <v>2.1</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="14"/>
@@ -3008,19 +2985,19 @@
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <f ca="1">COUNTA(OFFSET(tblPlan[[#Headers],[Task]],1,0,ROW()-1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" s="12">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6" s="13" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>1.4</v>
+        <v>2.2</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="14"/>
@@ -3037,21 +3014,21 @@
       <c r="K6" s="24"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="21">
+      <c r="A7" s="11">
         <f ca="1">COUNTA(OFFSET(tblPlan[[#Headers],[Task]],1,0,ROW()-1))</f>
-        <v>1</v>
-      </c>
-      <c r="B7" s="22">
+        <v>2</v>
+      </c>
+      <c r="B7" s="12">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>5</v>
-      </c>
-      <c r="C7" s="23" t="str">
+        <v>3</v>
+      </c>
+      <c r="C7" s="13" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>1.5</v>
+        <v>2.3</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="14"/>
@@ -3059,8 +3036,12 @@
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",MAX(OFFSET(tblPlan[[#This Row],[Start]],1,1,COUNTIF(tblPlan[Lv1.],tblPlan[[#This Row],[Lv1.]])-1)),IF(tblPlan[[#This Row],[Start]]&lt;&gt;"",WORKDAY.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Efforts(mds)]]-NETWORKDAYS.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Start]],11,tblHoliday[Date]),11,tblHoliday[Date]),""))</f>
         <v/>
       </c>
-      <c r="I7" s="16"/>
-      <c r="J7" s="26"/>
+      <c r="I7" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="26">
+        <v>0</v>
+      </c>
       <c r="K7" s="24"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -3070,55 +3051,55 @@
       </c>
       <c r="B8" s="12">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>0</v>
-      </c>
-      <c r="C8" s="13">
+        <v>4</v>
+      </c>
+      <c r="C8" s="13" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>2</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="9"/>
+        <v>2.4</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9" t="s">
+        <v>74</v>
+      </c>
       <c r="F8" s="9"/>
       <c r="G8" s="14"/>
-      <c r="H8" s="15">
+      <c r="H8" s="15" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",MAX(OFFSET(tblPlan[[#This Row],[Start]],1,1,COUNTIF(tblPlan[Lv1.],tblPlan[[#This Row],[Lv1.]])-1)),IF(tblPlan[[#This Row],[Start]]&lt;&gt;"",WORKDAY.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Efforts(mds)]]-NETWORKDAYS.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Start]],11,tblHoliday[Date]),11,tblHoliday[Date]),""))</f>
+        <v/>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="26">
         <v>0</v>
       </c>
-      <c r="I8" s="16"/>
-      <c r="J8" s="26"/>
       <c r="K8" s="24"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <f ca="1">COUNTA(OFFSET(tblPlan[[#Headers],[Task]],1,0,ROW()-1))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9" s="12">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>1</v>
-      </c>
-      <c r="C9" s="13" t="str">
+        <v>0</v>
+      </c>
+      <c r="C9" s="13">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>2.1</v>
-      </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9" t="s">
-        <v>54</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="14"/>
-      <c r="H9" s="15" t="str">
+      <c r="H9" s="15">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",MAX(OFFSET(tblPlan[[#This Row],[Start]],1,1,COUNTIF(tblPlan[Lv1.],tblPlan[[#This Row],[Lv1.]])-1)),IF(tblPlan[[#This Row],[Start]]&lt;&gt;"",WORKDAY.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Efforts(mds)]]-NETWORKDAYS.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Start]],11,tblHoliday[Date]),11,tblHoliday[Date]),""))</f>
-        <v/>
-      </c>
-      <c r="I9" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="J9" s="26">
-        <v>0.8</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I9" s="16"/>
+      <c r="J9" s="26"/>
       <c r="K9" s="24"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -3128,42 +3109,46 @@
       </c>
       <c r="B10" s="12">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>0</v>
-      </c>
-      <c r="C10" s="13">
+        <v>1</v>
+      </c>
+      <c r="C10" s="13" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>3</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="9"/>
+        <v>3.1</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9" t="s">
+        <v>48</v>
+      </c>
       <c r="F10" s="9"/>
       <c r="G10" s="14"/>
-      <c r="H10" s="15">
+      <c r="H10" s="15" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",MAX(OFFSET(tblPlan[[#This Row],[Start]],1,1,COUNTIF(tblPlan[Lv1.],tblPlan[[#This Row],[Lv1.]])-1)),IF(tblPlan[[#This Row],[Start]]&lt;&gt;"",WORKDAY.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Efforts(mds)]]-NETWORKDAYS.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Start]],11,tblHoliday[Date]),11,tblHoliday[Date]),""))</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="16"/>
-      <c r="J10" s="26"/>
+        <v/>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" s="26">
+        <v>1</v>
+      </c>
       <c r="K10" s="24"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="11">
+      <c r="A11" s="21">
         <f ca="1">COUNTA(OFFSET(tblPlan[[#Headers],[Task]],1,0,ROW()-1))</f>
         <v>3</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="22">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>1</v>
-      </c>
-      <c r="C11" s="13" t="str">
+        <v>2</v>
+      </c>
+      <c r="C11" s="23" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="14"/>
@@ -3172,7 +3157,7 @@
         <v/>
       </c>
       <c r="I11" s="16" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="J11" s="26">
         <v>1</v>
@@ -3186,15 +3171,15 @@
       </c>
       <c r="B12" s="22">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12" s="23" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="14"/>
@@ -3203,7 +3188,7 @@
         <v/>
       </c>
       <c r="I12" s="16" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="J12" s="26">
         <v>1</v>
@@ -3211,21 +3196,21 @@
       <c r="K12" s="24"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="11">
+      <c r="A13" s="21">
         <f ca="1">COUNTA(OFFSET(tblPlan[[#Headers],[Task]],1,0,ROW()-1))</f>
         <v>3</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="22">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>3</v>
-      </c>
-      <c r="C13" s="13" t="str">
+        <v>4</v>
+      </c>
+      <c r="C13" s="23" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="14"/>
@@ -3234,10 +3219,10 @@
         <v/>
       </c>
       <c r="I13" s="16" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="J13" s="26">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="K13" s="24"/>
     </row>
@@ -3248,15 +3233,15 @@
       </c>
       <c r="B14" s="22">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14" s="23" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="14"/>
@@ -3265,38 +3250,42 @@
         <v/>
       </c>
       <c r="I14" s="16" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="J14" s="26">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="K14" s="24"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="11">
+      <c r="A15" s="21">
         <f ca="1">COUNTA(OFFSET(tblPlan[[#Headers],[Task]],1,0,ROW()-1))</f>
-        <v>4</v>
-      </c>
-      <c r="B15" s="12">
+        <v>3</v>
+      </c>
+      <c r="B15" s="22">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>0</v>
-      </c>
-      <c r="C15" s="13">
+        <v>6</v>
+      </c>
+      <c r="C15" s="23" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>4</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="9"/>
+        <v>3.6</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9" t="s">
+        <v>52</v>
+      </c>
       <c r="F15" s="9"/>
       <c r="G15" s="14"/>
-      <c r="H15" s="15">
+      <c r="H15" s="15" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",MAX(OFFSET(tblPlan[[#This Row],[Start]],1,1,COUNTIF(tblPlan[Lv1.],tblPlan[[#This Row],[Lv1.]])-1)),IF(tblPlan[[#This Row],[Start]]&lt;&gt;"",WORKDAY.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Efforts(mds)]]-NETWORKDAYS.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Start]],11,tblHoliday[Date]),11,tblHoliday[Date]),""))</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="16"/>
-      <c r="J15" s="26"/>
+        <v/>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J15" s="26">
+        <v>0.7</v>
+      </c>
       <c r="K15" s="24"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -3306,28 +3295,24 @@
       </c>
       <c r="B16" s="12">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>1</v>
-      </c>
-      <c r="C16" s="13" t="str">
+        <v>0</v>
+      </c>
+      <c r="C16" s="13">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>4.1</v>
-      </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9" t="s">
-        <v>61</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="14"/>
-      <c r="H16" s="15" t="str">
+      <c r="H16" s="15">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",MAX(OFFSET(tblPlan[[#This Row],[Start]],1,1,COUNTIF(tblPlan[Lv1.],tblPlan[[#This Row],[Lv1.]])-1)),IF(tblPlan[[#This Row],[Start]]&lt;&gt;"",WORKDAY.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Efforts(mds)]]-NETWORKDAYS.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Start]],11,tblHoliday[Date]),11,tblHoliday[Date]),""))</f>
-        <v/>
-      </c>
-      <c r="I16" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="J16" s="26">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I16" s="16"/>
+      <c r="J16" s="26"/>
       <c r="K16" s="24"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -3337,15 +3322,15 @@
       </c>
       <c r="B17" s="12">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" s="13" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>4.2</v>
+        <v>4.1</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="14"/>
@@ -3354,7 +3339,7 @@
         <v/>
       </c>
       <c r="I17" s="16" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="J17" s="26">
         <v>1</v>
@@ -3362,21 +3347,21 @@
       <c r="K17" s="24"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="11">
+      <c r="A18" s="21">
         <f ca="1">COUNTA(OFFSET(tblPlan[[#Headers],[Task]],1,0,ROW()-1))</f>
         <v>4</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="22">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>3</v>
-      </c>
-      <c r="C18" s="13" t="str">
+        <v>2</v>
+      </c>
+      <c r="C18" s="23" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>4.3</v>
+        <v>4.2</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="14"/>
@@ -3385,29 +3370,29 @@
         <v/>
       </c>
       <c r="I18" s="16" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="J18" s="26">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="K18" s="24"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="11">
+      <c r="A19" s="21">
         <f ca="1">COUNTA(OFFSET(tblPlan[[#Headers],[Task]],1,0,ROW()-1))</f>
         <v>4</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B19" s="22">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>4</v>
-      </c>
-      <c r="C19" s="13" t="str">
+        <v>3</v>
+      </c>
+      <c r="C19" s="23" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>4.4</v>
+        <v>4.3</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="14"/>
@@ -3416,29 +3401,29 @@
         <v/>
       </c>
       <c r="I19" s="16" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="J19" s="26">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K19" s="24"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="11">
+      <c r="A20" s="21">
         <f ca="1">COUNTA(OFFSET(tblPlan[[#Headers],[Task]],1,0,ROW()-1))</f>
         <v>4</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B20" s="22">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>5</v>
-      </c>
-      <c r="C20" s="13" t="str">
+        <v>4</v>
+      </c>
+      <c r="C20" s="23" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>4.5</v>
+        <v>4.4</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="14"/>
@@ -3447,60 +3432,56 @@
         <v/>
       </c>
       <c r="I20" s="16" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="J20" s="26">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K20" s="24"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <f ca="1">COUNTA(OFFSET(tblPlan[[#Headers],[Task]],1,0,ROW()-1))</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B21" s="12">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>6</v>
-      </c>
-      <c r="C21" s="13" t="str">
+        <v>0</v>
+      </c>
+      <c r="C21" s="13">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>4.6</v>
-      </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9" t="s">
-        <v>67</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="14"/>
-      <c r="H21" s="15" t="str">
+      <c r="H21" s="15">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",MAX(OFFSET(tblPlan[[#This Row],[Start]],1,1,COUNTIF(tblPlan[Lv1.],tblPlan[[#This Row],[Lv1.]])-1)),IF(tblPlan[[#This Row],[Start]]&lt;&gt;"",WORKDAY.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Efforts(mds)]]-NETWORKDAYS.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Start]],11,tblHoliday[Date]),11,tblHoliday[Date]),""))</f>
-        <v/>
-      </c>
-      <c r="I21" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="J21" s="26">
         <v>0</v>
       </c>
+      <c r="I21" s="16"/>
+      <c r="J21" s="26"/>
       <c r="K21" s="24"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
         <f ca="1">COUNTA(OFFSET(tblPlan[[#Headers],[Task]],1,0,ROW()-1))</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B22" s="12">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C22" s="13" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>4.7</v>
+        <v>5.1</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="14"/>
@@ -3509,10 +3490,10 @@
         <v/>
       </c>
       <c r="I22" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J22" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" s="24"/>
     </row>
@@ -3523,24 +3504,28 @@
       </c>
       <c r="B23" s="12">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>0</v>
-      </c>
-      <c r="C23" s="13">
+        <v>2</v>
+      </c>
+      <c r="C23" s="13" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>5</v>
-      </c>
-      <c r="D23" s="9" t="s">
+        <v>5.2</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="14"/>
-      <c r="H23" s="15">
+      <c r="H23" s="15" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",MAX(OFFSET(tblPlan[[#This Row],[Start]],1,1,COUNTIF(tblPlan[Lv1.],tblPlan[[#This Row],[Lv1.]])-1)),IF(tblPlan[[#This Row],[Start]]&lt;&gt;"",WORKDAY.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Efforts(mds)]]-NETWORKDAYS.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Start]],11,tblHoliday[Date]),11,tblHoliday[Date]),""))</f>
-        <v>0</v>
-      </c>
-      <c r="I23" s="16"/>
-      <c r="J23" s="26"/>
+        <v/>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="J23" s="26">
+        <v>1</v>
+      </c>
       <c r="K23" s="24"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -3550,15 +3535,15 @@
       </c>
       <c r="B24" s="12">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C24" s="13" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>5.1</v>
+        <v>5.3</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="14"/>
@@ -3567,7 +3552,7 @@
         <v/>
       </c>
       <c r="I24" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J24" s="26">
         <v>1</v>
@@ -3581,15 +3566,15 @@
       </c>
       <c r="B25" s="12">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C25" s="13" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>5.2</v>
+        <v>5.4</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="14"/>
@@ -3598,10 +3583,10 @@
         <v/>
       </c>
       <c r="I25" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J25" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25" s="24"/>
     </row>
@@ -3612,15 +3597,15 @@
       </c>
       <c r="B26" s="12">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C26" s="13" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>5.3</v>
+        <v>5.5</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="14"/>
@@ -3629,7 +3614,7 @@
         <v/>
       </c>
       <c r="I26" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J26" s="26">
         <v>1</v>
@@ -3643,15 +3628,15 @@
       </c>
       <c r="B27" s="12">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C27" s="13" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>5.4</v>
+        <v>5.6</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="14"/>
@@ -3660,7 +3645,7 @@
         <v/>
       </c>
       <c r="I27" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J27" s="26">
         <v>1</v>
@@ -3674,15 +3659,15 @@
       </c>
       <c r="B28" s="12">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C28" s="13" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>5.5</v>
+        <v>5.7</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="14"/>
@@ -3691,10 +3676,10 @@
         <v/>
       </c>
       <c r="I28" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J28" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K28" s="24"/>
     </row>
@@ -3705,15 +3690,15 @@
       </c>
       <c r="B29" s="22">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C29" s="23" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>5.6</v>
+        <v>5.8</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="9" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="14"/>
@@ -3722,7 +3707,7 @@
         <v/>
       </c>
       <c r="I29" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J29" s="26">
         <v>0</v>
@@ -3743,7 +3728,7 @@
         <v>6</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
@@ -3771,7 +3756,7 @@
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="F31" s="9"/>
       <c r="G31" s="14"/>
@@ -3780,10 +3765,10 @@
         <v/>
       </c>
       <c r="I31" s="16" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="J31" s="26">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="K31" s="24"/>
     </row>
@@ -3802,7 +3787,7 @@
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="F32" s="9"/>
       <c r="G32" s="14"/>
@@ -3811,10 +3796,10 @@
         <v/>
       </c>
       <c r="I32" s="16" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="J32" s="26">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="K32" s="24"/>
     </row>
@@ -3833,7 +3818,7 @@
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="9" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="F33" s="9"/>
       <c r="G33" s="14"/>
@@ -3842,56 +3827,60 @@
         <v/>
       </c>
       <c r="I33" s="16" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="J33" s="26">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="K33" s="24"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="11">
         <f ca="1">COUNTA(OFFSET(tblPlan[[#Headers],[Task]],1,0,ROW()-1))</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B34" s="12">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>0</v>
-      </c>
-      <c r="C34" s="13">
+        <v>4</v>
+      </c>
+      <c r="C34" s="13" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>7</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E34" s="9"/>
+        <v>6.4</v>
+      </c>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9" t="s">
+        <v>52</v>
+      </c>
       <c r="F34" s="9"/>
       <c r="G34" s="14"/>
-      <c r="H34" s="15">
+      <c r="H34" s="15" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",MAX(OFFSET(tblPlan[[#This Row],[Start]],1,1,COUNTIF(tblPlan[Lv1.],tblPlan[[#This Row],[Lv1.]])-1)),IF(tblPlan[[#This Row],[Start]]&lt;&gt;"",WORKDAY.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Efforts(mds)]]-NETWORKDAYS.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Start]],11,tblHoliday[Date]),11,tblHoliday[Date]),""))</f>
+        <v/>
+      </c>
+      <c r="I34" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="J34" s="26">
         <v>0</v>
       </c>
-      <c r="I34" s="16"/>
-      <c r="J34" s="26"/>
       <c r="K34" s="24"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35" s="11">
+      <c r="A35" s="21">
         <f ca="1">COUNTA(OFFSET(tblPlan[[#Headers],[Task]],1,0,ROW()-1))</f>
-        <v>7</v>
-      </c>
-      <c r="B35" s="12">
+        <v>6</v>
+      </c>
+      <c r="B35" s="22">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>1</v>
-      </c>
-      <c r="C35" s="13" t="str">
+        <v>5</v>
+      </c>
+      <c r="C35" s="23" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>7.1</v>
+        <v>6.5</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="F35" s="9"/>
       <c r="G35" s="14"/>
@@ -3900,10 +3889,10 @@
         <v/>
       </c>
       <c r="I35" s="16" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="J35" s="26">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="K35" s="24"/>
     </row>
@@ -3914,73 +3903,73 @@
       </c>
       <c r="B36" s="12">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>2</v>
-      </c>
-      <c r="C36" s="13" t="str">
+        <v>0</v>
+      </c>
+      <c r="C36" s="13">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>7.2</v>
-      </c>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9" t="s">
-        <v>77</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E36" s="9"/>
       <c r="F36" s="9"/>
       <c r="G36" s="14"/>
-      <c r="H36" s="15" t="str">
+      <c r="H36" s="15">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",MAX(OFFSET(tblPlan[[#This Row],[Start]],1,1,COUNTIF(tblPlan[Lv1.],tblPlan[[#This Row],[Lv1.]])-1)),IF(tblPlan[[#This Row],[Start]]&lt;&gt;"",WORKDAY.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Efforts(mds)]]-NETWORKDAYS.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Start]],11,tblHoliday[Date]),11,tblHoliday[Date]),""))</f>
-        <v/>
-      </c>
-      <c r="I36" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="J36" s="26">
-        <v>0.8</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I36" s="16"/>
+      <c r="J36" s="26"/>
       <c r="K36" s="24"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="11">
         <f ca="1">COUNTA(OFFSET(tblPlan[[#Headers],[Task]],1,0,ROW()-1))</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B37" s="12">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>0</v>
-      </c>
-      <c r="C37" s="13">
+        <v>1</v>
+      </c>
+      <c r="C37" s="13" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>8</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E37" s="9"/>
+        <v>7.1</v>
+      </c>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="F37" s="9"/>
       <c r="G37" s="14"/>
-      <c r="H37" s="15">
+      <c r="H37" s="15" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",MAX(OFFSET(tblPlan[[#This Row],[Start]],1,1,COUNTIF(tblPlan[Lv1.],tblPlan[[#This Row],[Lv1.]])-1)),IF(tblPlan[[#This Row],[Start]]&lt;&gt;"",WORKDAY.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Efforts(mds)]]-NETWORKDAYS.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Start]],11,tblHoliday[Date]),11,tblHoliday[Date]),""))</f>
-        <v>0</v>
-      </c>
-      <c r="I37" s="16"/>
-      <c r="J37" s="26"/>
+        <v/>
+      </c>
+      <c r="I37" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J37" s="26">
+        <v>1</v>
+      </c>
       <c r="K37" s="24"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="11">
         <f ca="1">COUNTA(OFFSET(tblPlan[[#Headers],[Task]],1,0,ROW()-1))</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B38" s="12">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C38" s="13" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>8.1</v>
+        <v>7.2</v>
       </c>
       <c r="D38" s="9"/>
       <c r="E38" s="9" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="F38" s="9"/>
       <c r="G38" s="14"/>
@@ -3992,26 +3981,26 @@
         <v>29</v>
       </c>
       <c r="J38" s="26">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="K38" s="24"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="11">
         <f ca="1">COUNTA(OFFSET(tblPlan[[#Headers],[Task]],1,0,ROW()-1))</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B39" s="12">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C39" s="13" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>8.2</v>
+        <v>7.3</v>
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="9" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="F39" s="9"/>
       <c r="G39" s="14"/>
@@ -4020,29 +4009,29 @@
         <v/>
       </c>
       <c r="I39" s="16" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="J39" s="26">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="K39" s="24"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40" s="11">
+      <c r="A40" s="21">
         <f ca="1">COUNTA(OFFSET(tblPlan[[#Headers],[Task]],1,0,ROW()-1))</f>
-        <v>8</v>
-      </c>
-      <c r="B40" s="12">
+        <v>7</v>
+      </c>
+      <c r="B40" s="22">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>3</v>
-      </c>
-      <c r="C40" s="13" t="str">
+        <v>4</v>
+      </c>
+      <c r="C40" s="23" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>8.3</v>
+        <v>7.4</v>
       </c>
       <c r="D40" s="9"/>
       <c r="E40" s="9" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="F40" s="9"/>
       <c r="G40" s="14"/>
@@ -4051,10 +4040,10 @@
         <v/>
       </c>
       <c r="I40" s="16" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="J40" s="26">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="K40" s="24"/>
     </row>
@@ -4065,46 +4054,42 @@
       </c>
       <c r="B41" s="12">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>4</v>
-      </c>
-      <c r="C41" s="13" t="str">
+        <v>0</v>
+      </c>
+      <c r="C41" s="13">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>8.4</v>
-      </c>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9" t="s">
-        <v>81</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E41" s="9"/>
       <c r="F41" s="9"/>
       <c r="G41" s="14"/>
-      <c r="H41" s="15" t="str">
+      <c r="H41" s="15">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",MAX(OFFSET(tblPlan[[#This Row],[Start]],1,1,COUNTIF(tblPlan[Lv1.],tblPlan[[#This Row],[Lv1.]])-1)),IF(tblPlan[[#This Row],[Start]]&lt;&gt;"",WORKDAY.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Efforts(mds)]]-NETWORKDAYS.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Start]],11,tblHoliday[Date]),11,tblHoliday[Date]),""))</f>
-        <v/>
-      </c>
-      <c r="I41" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="J41" s="26">
-        <v>0.8</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I41" s="16"/>
+      <c r="J41" s="26"/>
       <c r="K41" s="24"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A42" s="21">
+      <c r="A42" s="11">
         <f ca="1">COUNTA(OFFSET(tblPlan[[#Headers],[Task]],1,0,ROW()-1))</f>
         <v>8</v>
       </c>
-      <c r="B42" s="22">
+      <c r="B42" s="12">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>5</v>
-      </c>
-      <c r="C42" s="23" t="str">
+        <v>1</v>
+      </c>
+      <c r="C42" s="13" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>8.5</v>
+        <v>8.1</v>
       </c>
       <c r="D42" s="9"/>
       <c r="E42" s="9" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="F42" s="9"/>
       <c r="G42" s="14"/>
@@ -4112,35 +4097,43 @@
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",MAX(OFFSET(tblPlan[[#This Row],[Start]],1,1,COUNTIF(tblPlan[Lv1.],tblPlan[[#This Row],[Lv1.]])-1)),IF(tblPlan[[#This Row],[Start]]&lt;&gt;"",WORKDAY.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Efforts(mds)]]-NETWORKDAYS.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Start]],11,tblHoliday[Date]),11,tblHoliday[Date]),""))</f>
         <v/>
       </c>
-      <c r="I42" s="16"/>
-      <c r="J42" s="26"/>
+      <c r="I42" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="J42" s="26">
+        <v>0.8</v>
+      </c>
       <c r="K42" s="24"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A43" s="21">
+      <c r="A43" s="11">
         <f ca="1">COUNTA(OFFSET(tblPlan[[#Headers],[Task]],1,0,ROW()-1))</f>
-        <v>9</v>
-      </c>
-      <c r="B43" s="22">
+        <v>8</v>
+      </c>
+      <c r="B43" s="12">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>0</v>
-      </c>
-      <c r="C43" s="23">
+        <v>2</v>
+      </c>
+      <c r="C43" s="13" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>9</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E43" s="9"/>
+        <v>8.2</v>
+      </c>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9" t="s">
+        <v>65</v>
+      </c>
       <c r="F43" s="9"/>
       <c r="G43" s="14"/>
-      <c r="H43" s="15">
+      <c r="H43" s="15" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",MAX(OFFSET(tblPlan[[#This Row],[Start]],1,1,COUNTIF(tblPlan[Lv1.],tblPlan[[#This Row],[Lv1.]])-1)),IF(tblPlan[[#This Row],[Start]]&lt;&gt;"",WORKDAY.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Efforts(mds)]]-NETWORKDAYS.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Start]],11,tblHoliday[Date]),11,tblHoliday[Date]),""))</f>
-        <v>0</v>
-      </c>
-      <c r="I43" s="16"/>
-      <c r="J43" s="26"/>
+        <v/>
+      </c>
+      <c r="I43" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="J43" s="26">
+        <v>0.8</v>
+      </c>
       <c r="K43" s="24"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
@@ -4150,25 +4143,23 @@
       </c>
       <c r="B44" s="22">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>1</v>
-      </c>
-      <c r="C44" s="23" t="str">
+        <v>0</v>
+      </c>
+      <c r="C44" s="23">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>9.1</v>
-      </c>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9" t="s">
-        <v>82</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E44" s="9"/>
       <c r="F44" s="9"/>
       <c r="G44" s="14"/>
-      <c r="H44" s="15" t="str">
+      <c r="H44" s="15">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",MAX(OFFSET(tblPlan[[#This Row],[Start]],1,1,COUNTIF(tblPlan[Lv1.],tblPlan[[#This Row],[Lv1.]])-1)),IF(tblPlan[[#This Row],[Start]]&lt;&gt;"",WORKDAY.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Efforts(mds)]]-NETWORKDAYS.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Start]],11,tblHoliday[Date]),11,tblHoliday[Date]),""))</f>
-        <v/>
-      </c>
-      <c r="I44" s="16" t="s">
-        <v>34</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I44" s="16"/>
       <c r="J44" s="26">
         <v>1</v>
       </c>
@@ -4181,15 +4172,15 @@
       </c>
       <c r="B45" s="22">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C45" s="23" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>9.2</v>
+        <v>9.1</v>
       </c>
       <c r="D45" s="9"/>
       <c r="E45" s="9" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="F45" s="9"/>
       <c r="G45" s="14"/>
@@ -4198,170 +4189,77 @@
         <v/>
       </c>
       <c r="I45" s="16" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="J45" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K45" s="24"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="21">
         <f ca="1">COUNTA(OFFSET(tblPlan[[#Headers],[Task]],1,0,ROW()-1))</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B46" s="22">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>0</v>
-      </c>
-      <c r="C46" s="23">
+        <v>2</v>
+      </c>
+      <c r="C46" s="23" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>10</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>48</v>
-      </c>
+        <v>9.2</v>
+      </c>
+      <c r="D46" s="9"/>
       <c r="E46" s="9"/>
       <c r="F46" s="9"/>
       <c r="G46" s="14"/>
-      <c r="H46" s="15">
+      <c r="H46" s="15" t="str">
         <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",MAX(OFFSET(tblPlan[[#This Row],[Start]],1,1,COUNTIF(tblPlan[Lv1.],tblPlan[[#This Row],[Lv1.]])-1)),IF(tblPlan[[#This Row],[Start]]&lt;&gt;"",WORKDAY.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Efforts(mds)]]-NETWORKDAYS.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Start]],11,tblHoliday[Date]),11,tblHoliday[Date]),""))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="I46" s="16"/>
       <c r="J46" s="26"/>
       <c r="K46" s="24"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" s="21">
-        <f ca="1">COUNTA(OFFSET(tblPlan[[#Headers],[Task]],1,0,ROW()-1))</f>
-        <v>10</v>
-      </c>
-      <c r="B47" s="22">
-        <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>1</v>
-      </c>
-      <c r="C47" s="23" t="str">
-        <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>10.1</v>
-      </c>
+      <c r="A47" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B47" s="9"/>
+      <c r="C47" s="17"/>
       <c r="D47" s="9"/>
-      <c r="E47" s="9" t="s">
-        <v>85</v>
-      </c>
+      <c r="E47" s="9"/>
       <c r="F47" s="9"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="15" t="str">
-        <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",MAX(OFFSET(tblPlan[[#This Row],[Start]],1,1,COUNTIF(tblPlan[Lv1.],tblPlan[[#This Row],[Lv1.]])-1)),IF(tblPlan[[#This Row],[Start]]&lt;&gt;"",WORKDAY.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Efforts(mds)]]-NETWORKDAYS.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Start]],11,tblHoliday[Date]),11,tblHoliday[Date]),""))</f>
-        <v/>
-      </c>
-      <c r="I47" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="J47" s="26">
-        <v>1</v>
-      </c>
-      <c r="K47" s="24"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48" s="21">
-        <f ca="1">COUNTA(OFFSET(tblPlan[[#Headers],[Task]],1,0,ROW()-1))</f>
-        <v>10</v>
-      </c>
-      <c r="B48" s="22">
-        <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>2</v>
-      </c>
-      <c r="C48" s="23" t="str">
-        <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>10.2</v>
-      </c>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="F48" s="9"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="15" t="str">
-        <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",MAX(OFFSET(tblPlan[[#This Row],[Start]],1,1,COUNTIF(tblPlan[Lv1.],tblPlan[[#This Row],[Lv1.]])-1)),IF(tblPlan[[#This Row],[Start]]&lt;&gt;"",WORKDAY.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Efforts(mds)]]-NETWORKDAYS.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Start]],11,tblHoliday[Date]),11,tblHoliday[Date]),""))</f>
-        <v/>
-      </c>
-      <c r="I48" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="J48" s="26">
-        <v>0</v>
-      </c>
-      <c r="K48" s="24"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A49" s="21">
-        <f ca="1">COUNTA(OFFSET(tblPlan[[#Headers],[Task]],1,0,ROW()-1))</f>
-        <v>10</v>
-      </c>
-      <c r="B49" s="22">
-        <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",0,OFFSET(tblPlan[[#This Row],[No.]],-1,-1)+1)</f>
-        <v>3</v>
-      </c>
-      <c r="C49" s="23" t="str">
-        <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",tblPlan[[#This Row],[Lv1.]],tblPlan[[#This Row],[Lv1.]]&amp;"."&amp;tblPlan[[#This Row],[Lv2.]])</f>
-        <v>10.3</v>
-      </c>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F49" s="9"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="15" t="str">
-        <f ca="1">IF(tblPlan[[#This Row],[Task]]&lt;&gt;"",MAX(OFFSET(tblPlan[[#This Row],[Start]],1,1,COUNTIF(tblPlan[Lv1.],tblPlan[[#This Row],[Lv1.]])-1)),IF(tblPlan[[#This Row],[Start]]&lt;&gt;"",WORKDAY.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Efforts(mds)]]-NETWORKDAYS.INTL(tblPlan[[#This Row],[Start]],tblPlan[[#This Row],[Start]],11,tblHoliday[Date]),11,tblHoliday[Date]),""))</f>
-        <v/>
-      </c>
-      <c r="I49" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="J49" s="26"/>
-      <c r="K49" s="24"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B50" s="9"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="14">
+      <c r="G47" s="9"/>
+      <c r="H47" s="14">
         <f ca="1">SUBTOTAL(104,tblPlan[Finish])</f>
         <v>0</v>
       </c>
-      <c r="I50" s="9"/>
-      <c r="J50" s="9"/>
-      <c r="K50" s="10"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H53" s="25"/>
-      <c r="I53" s="25"/>
-      <c r="J53" s="25"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H54" s="25"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+      <c r="K47" s="10"/>
+    </row>
+    <row r="50" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H50" s="25"/>
+      <c r="I50" s="25"/>
+      <c r="J50" s="25"/>
+    </row>
+    <row r="51" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H51" s="25"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="Ff3/vy1CQrWHbK51b9erxfPJIfA9yIq1fM0vUqD2JEsYJWpckJc9+mMkyiNBR0kjDnLJbSXiOYeD75PhSZSp5w==" saltValue="B1FBsWn82PA8znCP9LieZw==" spinCount="100000" sheet="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <conditionalFormatting sqref="A21:J21 A2:K20 A22:K32 A33:J34 A35:K49">
-    <cfRule type="expression" dxfId="2" priority="6">
-      <formula>$D2&lt;&gt;""</formula>
+  <conditionalFormatting sqref="A27:J27 A39:J41 A42:K46 A28:K38 A4:K26">
+    <cfRule type="expression" dxfId="13" priority="6">
+      <formula>$D4&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G49">
-    <cfRule type="expression" dxfId="1" priority="5">
+  <conditionalFormatting sqref="G2:G46">
+    <cfRule type="expression" dxfId="12" priority="5">
       <formula>AND($G2&lt;&gt;"",WEEKDAY($G2,2)&gt;=6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J49">
+  <conditionalFormatting sqref="J2:J46">
     <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4375,19 +4273,19 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K21">
-    <cfRule type="expression" dxfId="0" priority="2">
-      <formula>$D17&lt;&gt;""</formula>
+  <conditionalFormatting sqref="K27">
+    <cfRule type="expression" dxfId="11" priority="2">
+      <formula>$D23&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G49" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G46" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>32874</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I49" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I46" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>INDIRECT("tblResources[Account]")</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J49" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J46" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -4395,7 +4293,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="C49 C43 A15:C20 A8:C11 A2:C6 A13:C13 A21:C28 A30:C33 A34:C36 A37:C41" unlockedFormula="1"/>
+    <ignoredError sqref="C46 A16:C17 A41:C43 A21:C28 A36:C39 A30:C34 A4:C10" unlockedFormula="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
@@ -4416,7 +4314,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>J2:J49</xm:sqref>
+          <xm:sqref>J2:J46</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4480,10 +4378,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4527,25 +4425,12 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
-        <f>ROW()-ROW(tblResources[[#Headers],[No.]])</f>
-        <v>3</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>